<commit_message>
Updated data from Cannabis Commission
</commit_message>
<xml_diff>
--- a/State Application Process Data New.xlsx
+++ b/State Application Process Data New.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeppl\Google Drive\Terpene Journey\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeppl\Documents\dataprojects\masscannabis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC290FCE-37AD-45E8-9831-01CDF517D864}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6E7187D4-068C-4C16-970B-449788BF71A5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5230" xr2:uid="{85ECA81A-E34F-418E-A48A-9CD5C15FB6EE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5230" activeTab="1" xr2:uid="{85ECA81A-E34F-418E-A48A-9CD5C15FB6EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="underReview" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>totalApps</t>
   </si>
@@ -64,6 +65,12 @@
   </si>
   <si>
     <t>transporter</t>
+  </si>
+  <si>
+    <t>appsReview</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -416,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972E11FE-47D4-4AB3-97F6-C4CA662706D9}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -673,6 +680,129 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>43256</v>
+      </c>
+      <c r="B7">
+        <v>1002</v>
+      </c>
+      <c r="C7">
+        <v>108</v>
+      </c>
+      <c r="D7">
+        <v>61</v>
+      </c>
+      <c r="E7">
+        <v>833</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>30</v>
+      </c>
+      <c r="H7">
+        <v>22</v>
+      </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>14</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+      <c r="L7">
+        <v>30</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA1CB1F9-3C0F-49BE-91E7-5775A73E9F00}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>43256</v>
+      </c>
+      <c r="B2">
+        <v>51</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>15</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Uploaded new weekly data update
</commit_message>
<xml_diff>
--- a/State Application Process Data New.xlsx
+++ b/State Application Process Data New.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeppl\Documents\dataprojects\masscannabis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6E7187D4-068C-4C16-970B-449788BF71A5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{004AED9D-EE4B-4AC5-82B7-87370907C365}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5230" activeTab="1" xr2:uid="{85ECA81A-E34F-418E-A48A-9CD5C15FB6EE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5230" xr2:uid="{85ECA81A-E34F-418E-A48A-9CD5C15FB6EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>totalApps</t>
   </si>
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972E11FE-47D4-4AB3-97F6-C4CA662706D9}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:M1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -721,6 +721,47 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>43265</v>
+      </c>
+      <c r="B8">
+        <v>1145</v>
+      </c>
+      <c r="C8">
+        <v>128</v>
+      </c>
+      <c r="D8">
+        <v>72</v>
+      </c>
+      <c r="E8">
+        <v>945</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>34</v>
+      </c>
+      <c r="H8">
+        <v>26</v>
+      </c>
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8">
+        <v>17</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+      <c r="L8">
+        <v>36</v>
+      </c>
+      <c r="M8">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -728,14 +769,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA1CB1F9-3C0F-49BE-91E7-5775A73E9F00}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -803,6 +845,38 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>43265</v>
+      </c>
+      <c r="B3">
+        <v>53</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>12</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>17</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>